<commit_message>
credito por debito en TC_002
</commit_message>
<xml_diff>
--- a/Practico/Trabajos Practicos/TP12/TP12_CasosDePrueba.xlsx
+++ b/Practico/Trabajos Practicos/TP12/TP12_CasosDePrueba.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Facu\4\ISW\ISW_G9\Practico\Trabajos Practicos\TP12\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{836EDCEE-22B0-4FE2-843A-B0CD13B01FA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0612E63C-9DB7-4EAE-82B4-F2F999B1A8A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -805,9 +805,6 @@
     <t>1,2,3,4,5,6,8,9,10,11,12,13,14,15,16,17</t>
   </si>
   <si>
-    <t>Realizar pedido para envio con fecha especifica y pago con tarjeta de debito MasterCard.</t>
-  </si>
-  <si>
     <t>•usuario "Facundito" logueado con permiso de cliente.
 •ciudades "Córdoba, Villa Gral Belgrano, San Francisco" cargadas.
 •Comercio "McDonalds" cargado en el carrito de compra.
@@ -832,6 +829,9 @@
   </si>
   <si>
     <t>Realizar pedido para envio lo antes posible y pago efectivo, con calle no existente y ciudad no cubierta por el servicio.</t>
+  </si>
+  <si>
+    <t>Realizar pedido para envio con fecha especifica y pago con tarjeta de crédito MasterCard.</t>
   </si>
 </sst>
 </file>
@@ -1649,28 +1649,13 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="8" fillId="8" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="8" fillId="8" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="6" fillId="10" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1680,8 +1665,23 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="8" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2743,7 +2743,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
+      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2818,26 +2818,26 @@
       <c r="AP1" s="28"/>
     </row>
     <row r="2" spans="1:42" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="97" t="s">
+      <c r="A2" s="87" t="s">
         <v>75</v>
       </c>
-      <c r="B2" s="98"/>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="98"/>
-      <c r="F2" s="98"/>
-      <c r="G2" s="90"/>
-      <c r="H2" s="91"/>
-      <c r="I2" s="91"/>
-      <c r="J2" s="91"/>
-      <c r="K2" s="91"/>
-      <c r="L2" s="91"/>
-      <c r="M2" s="90"/>
-      <c r="N2" s="91"/>
-      <c r="O2" s="91"/>
-      <c r="P2" s="91"/>
-      <c r="Q2" s="91"/>
-      <c r="R2" s="91"/>
+      <c r="B2" s="88"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="102"/>
+      <c r="H2" s="103"/>
+      <c r="I2" s="103"/>
+      <c r="J2" s="103"/>
+      <c r="K2" s="103"/>
+      <c r="L2" s="103"/>
+      <c r="M2" s="102"/>
+      <c r="N2" s="103"/>
+      <c r="O2" s="103"/>
+      <c r="P2" s="103"/>
+      <c r="Q2" s="103"/>
+      <c r="R2" s="103"/>
       <c r="S2" s="72"/>
       <c r="T2" s="72"/>
       <c r="U2" s="72"/>
@@ -2864,24 +2864,24 @@
       <c r="AP2" s="28"/>
     </row>
     <row r="3" spans="1:42" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="99"/>
-      <c r="B3" s="100"/>
-      <c r="C3" s="100"/>
-      <c r="D3" s="100"/>
-      <c r="E3" s="100"/>
-      <c r="F3" s="92"/>
-      <c r="G3" s="92"/>
-      <c r="H3" s="93"/>
-      <c r="I3" s="93"/>
-      <c r="J3" s="93"/>
-      <c r="K3" s="93"/>
-      <c r="L3" s="92"/>
-      <c r="M3" s="92"/>
-      <c r="N3" s="93"/>
-      <c r="O3" s="93"/>
-      <c r="P3" s="93"/>
-      <c r="Q3" s="93"/>
-      <c r="R3" s="92"/>
+      <c r="A3" s="89"/>
+      <c r="B3" s="90"/>
+      <c r="C3" s="90"/>
+      <c r="D3" s="90"/>
+      <c r="E3" s="90"/>
+      <c r="F3" s="91"/>
+      <c r="G3" s="91"/>
+      <c r="H3" s="104"/>
+      <c r="I3" s="104"/>
+      <c r="J3" s="104"/>
+      <c r="K3" s="104"/>
+      <c r="L3" s="91"/>
+      <c r="M3" s="91"/>
+      <c r="N3" s="104"/>
+      <c r="O3" s="104"/>
+      <c r="P3" s="104"/>
+      <c r="Q3" s="104"/>
+      <c r="R3" s="91"/>
       <c r="S3" s="74"/>
       <c r="T3" s="74"/>
       <c r="U3" s="74"/>
@@ -2908,24 +2908,24 @@
       <c r="AP3" s="28"/>
     </row>
     <row r="4" spans="1:42" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="101"/>
-      <c r="B4" s="102"/>
-      <c r="C4" s="92"/>
-      <c r="D4" s="92"/>
-      <c r="E4" s="92"/>
-      <c r="F4" s="92"/>
-      <c r="G4" s="92"/>
-      <c r="H4" s="92"/>
-      <c r="I4" s="92"/>
-      <c r="J4" s="94"/>
-      <c r="K4" s="94"/>
-      <c r="L4" s="94"/>
-      <c r="M4" s="94"/>
-      <c r="N4" s="94"/>
-      <c r="O4" s="94"/>
-      <c r="P4" s="94"/>
-      <c r="Q4" s="94"/>
-      <c r="R4" s="94"/>
+      <c r="A4" s="92"/>
+      <c r="B4" s="93"/>
+      <c r="C4" s="91"/>
+      <c r="D4" s="91"/>
+      <c r="E4" s="91"/>
+      <c r="F4" s="91"/>
+      <c r="G4" s="91"/>
+      <c r="H4" s="91"/>
+      <c r="I4" s="91"/>
+      <c r="J4" s="105"/>
+      <c r="K4" s="105"/>
+      <c r="L4" s="105"/>
+      <c r="M4" s="105"/>
+      <c r="N4" s="105"/>
+      <c r="O4" s="105"/>
+      <c r="P4" s="105"/>
+      <c r="Q4" s="105"/>
+      <c r="R4" s="105"/>
       <c r="S4" s="76"/>
       <c r="T4" s="76"/>
       <c r="U4" s="76"/>
@@ -2952,19 +2952,19 @@
       <c r="AP4" s="28"/>
     </row>
     <row r="5" spans="1:42" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="103" t="s">
+      <c r="A5" s="94" t="s">
         <v>76</v>
       </c>
-      <c r="B5" s="104"/>
+      <c r="B5" s="95"/>
       <c r="C5" s="78" t="s">
         <v>204</v>
       </c>
-      <c r="D5" s="105"/>
-      <c r="E5" s="96"/>
-      <c r="F5" s="96"/>
-      <c r="G5" s="95"/>
-      <c r="H5" s="96"/>
-      <c r="I5" s="96"/>
+      <c r="D5" s="96"/>
+      <c r="E5" s="97"/>
+      <c r="F5" s="97"/>
+      <c r="G5" s="106"/>
+      <c r="H5" s="97"/>
+      <c r="I5" s="97"/>
       <c r="J5" s="30"/>
       <c r="K5" s="30"/>
       <c r="L5" s="30"/>
@@ -3088,34 +3088,34 @@
       <c r="AP7" s="28"/>
     </row>
     <row r="8" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A8" s="106"/>
-      <c r="B8" s="88"/>
-      <c r="C8" s="88"/>
-      <c r="D8" s="88"/>
-      <c r="E8" s="88"/>
-      <c r="F8" s="88"/>
-      <c r="G8" s="89"/>
-      <c r="H8" s="87" t="s">
+      <c r="A8" s="98"/>
+      <c r="B8" s="99"/>
+      <c r="C8" s="99"/>
+      <c r="D8" s="99"/>
+      <c r="E8" s="99"/>
+      <c r="F8" s="99"/>
+      <c r="G8" s="100"/>
+      <c r="H8" s="101" t="s">
         <v>77</v>
       </c>
-      <c r="I8" s="88"/>
-      <c r="J8" s="88"/>
-      <c r="K8" s="88"/>
-      <c r="L8" s="89"/>
-      <c r="M8" s="87" t="s">
+      <c r="I8" s="99"/>
+      <c r="J8" s="99"/>
+      <c r="K8" s="99"/>
+      <c r="L8" s="100"/>
+      <c r="M8" s="101" t="s">
         <v>78</v>
       </c>
-      <c r="N8" s="88"/>
-      <c r="O8" s="88"/>
-      <c r="P8" s="88"/>
-      <c r="Q8" s="89"/>
-      <c r="R8" s="87" t="s">
+      <c r="N8" s="99"/>
+      <c r="O8" s="99"/>
+      <c r="P8" s="99"/>
+      <c r="Q8" s="100"/>
+      <c r="R8" s="101" t="s">
         <v>79</v>
       </c>
-      <c r="S8" s="88"/>
-      <c r="T8" s="88"/>
-      <c r="U8" s="88"/>
-      <c r="V8" s="89"/>
+      <c r="S8" s="99"/>
+      <c r="T8" s="99"/>
+      <c r="U8" s="99"/>
+      <c r="V8" s="100"/>
       <c r="W8" s="36"/>
       <c r="X8" s="36"/>
       <c r="Y8" s="36"/>
@@ -3283,7 +3283,7 @@
         <v>95</v>
       </c>
       <c r="E11" s="46" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F11" s="67" t="s">
         <v>96</v>
@@ -3340,10 +3340,10 @@
         <v>205</v>
       </c>
       <c r="D12" s="54" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="E12" s="55" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F12" s="67" t="s">
         <v>100</v>
@@ -3400,10 +3400,10 @@
         <v>94</v>
       </c>
       <c r="D13" s="54" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E13" s="54" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F13" s="70" t="s">
         <v>103</v>
@@ -3463,7 +3463,7 @@
         <v>106</v>
       </c>
       <c r="E14" s="46" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F14" s="67" t="s">
         <v>107</v>
@@ -3523,7 +3523,7 @@
         <v>110</v>
       </c>
       <c r="E15" s="46" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F15" s="67" t="s">
         <v>111</v>
@@ -3583,7 +3583,7 @@
         <v>114</v>
       </c>
       <c r="E16" s="46" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F16" s="67" t="s">
         <v>115</v>
@@ -3643,7 +3643,7 @@
         <v>118</v>
       </c>
       <c r="E17" s="46" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F17" s="67" t="s">
         <v>119</v>
@@ -3703,7 +3703,7 @@
         <v>123</v>
       </c>
       <c r="E18" s="46" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F18" s="67" t="s">
         <v>124</v>
@@ -3763,7 +3763,7 @@
         <v>128</v>
       </c>
       <c r="E19" s="46" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F19" s="68" t="s">
         <v>129</v>
@@ -3823,7 +3823,7 @@
         <v>132</v>
       </c>
       <c r="E20" s="46" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F20" s="68" t="s">
         <v>133</v>
@@ -3883,7 +3883,7 @@
         <v>136</v>
       </c>
       <c r="E21" s="58" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F21" s="68" t="s">
         <v>137</v>
@@ -3943,7 +3943,7 @@
         <v>140</v>
       </c>
       <c r="E22" s="46" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F22" s="67" t="s">
         <v>96</v>
@@ -4003,7 +4003,7 @@
         <v>144</v>
       </c>
       <c r="E23" s="46" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F23" s="67" t="s">
         <v>145</v>
@@ -47139,16 +47139,16 @@
   </sheetData>
   <autoFilter ref="A9:AP73" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <mergeCells count="10">
+    <mergeCell ref="M8:Q8"/>
+    <mergeCell ref="R8:V8"/>
+    <mergeCell ref="G2:L4"/>
+    <mergeCell ref="M2:R4"/>
+    <mergeCell ref="G5:I5"/>
     <mergeCell ref="A2:F4"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="D5:F5"/>
     <mergeCell ref="A8:G8"/>
     <mergeCell ref="H8:L8"/>
-    <mergeCell ref="M8:Q8"/>
-    <mergeCell ref="R8:V8"/>
-    <mergeCell ref="G2:L4"/>
-    <mergeCell ref="M2:R4"/>
-    <mergeCell ref="G5:I5"/>
   </mergeCells>
   <conditionalFormatting sqref="J9:J10 J12:J1000 J623:J1000 J749:J1000 J751:J1000 J753:J1000 J755:J1000 J757:J1000 J759:J1000 J761:J1000 J763:J1000 J765:J1000 J919:J1000 O9:O10 O12:O1000 O623:O1000 O749:O1000 O751:O1000 O753:O1000 O755:O1000 O757:O1000 O759:O1000 O761:O1000 O763:O1000 O765:O1000 O919:O1000">
     <cfRule type="cellIs" dxfId="46" priority="1" stopIfTrue="1" operator="equal">

</xml_diff>

<commit_message>
TP12 Bugs listo, revisar
</commit_message>
<xml_diff>
--- a/Practico/Trabajos Practicos/TP12/TP12_CasosDePrueba.xlsx
+++ b/Practico/Trabajos Practicos/TP12/TP12_CasosDePrueba.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Facu\4\ISW\ISW_G9\Practico\Trabajos Practicos\TP12\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0612E63C-9DB7-4EAE-82B4-F2F999B1A8A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14F628D3-6AED-4FB0-AF30-5D1B0D39BB43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="214">
   <si>
     <t>Número</t>
   </si>
@@ -833,6 +833,12 @@
   <si>
     <t>Realizar pedido para envio con fecha especifica y pago con tarjeta de crédito MasterCard.</t>
   </si>
+  <si>
+    <t>Paso</t>
+  </si>
+  <si>
+    <t>Fallo</t>
+  </si>
 </sst>
 </file>
 
@@ -1441,7 +1447,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1649,13 +1655,28 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="8" fillId="8" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="8" fillId="8" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="6" fillId="10" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1665,23 +1686,11 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="8" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="14" fontId="18" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2741,9 +2750,9 @@
   </sheetPr>
   <dimension ref="A1:AP1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
+      <selection pane="bottomLeft" activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2755,8 +2764,8 @@
     <col min="5" max="5" width="35.85546875" customWidth="1"/>
     <col min="6" max="6" width="48.28515625" customWidth="1"/>
     <col min="7" max="7" width="52" customWidth="1"/>
-    <col min="8" max="8" width="22" customWidth="1"/>
-    <col min="9" max="9" width="9.85546875" customWidth="1"/>
+    <col min="8" max="8" width="34.85546875" customWidth="1"/>
+    <col min="9" max="9" width="16" customWidth="1"/>
     <col min="10" max="10" width="19.5703125" customWidth="1"/>
     <col min="11" max="11" width="13.7109375" customWidth="1"/>
     <col min="12" max="12" width="12.42578125" customWidth="1"/>
@@ -2818,26 +2827,26 @@
       <c r="AP1" s="28"/>
     </row>
     <row r="2" spans="1:42" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="87" t="s">
+      <c r="A2" s="97" t="s">
         <v>75</v>
       </c>
-      <c r="B2" s="88"/>
-      <c r="C2" s="88"/>
-      <c r="D2" s="88"/>
-      <c r="E2" s="88"/>
-      <c r="F2" s="88"/>
-      <c r="G2" s="102"/>
-      <c r="H2" s="103"/>
-      <c r="I2" s="103"/>
-      <c r="J2" s="103"/>
-      <c r="K2" s="103"/>
-      <c r="L2" s="103"/>
-      <c r="M2" s="102"/>
-      <c r="N2" s="103"/>
-      <c r="O2" s="103"/>
-      <c r="P2" s="103"/>
-      <c r="Q2" s="103"/>
-      <c r="R2" s="103"/>
+      <c r="B2" s="98"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="91"/>
+      <c r="I2" s="91"/>
+      <c r="J2" s="91"/>
+      <c r="K2" s="91"/>
+      <c r="L2" s="91"/>
+      <c r="M2" s="90"/>
+      <c r="N2" s="91"/>
+      <c r="O2" s="91"/>
+      <c r="P2" s="91"/>
+      <c r="Q2" s="91"/>
+      <c r="R2" s="91"/>
       <c r="S2" s="72"/>
       <c r="T2" s="72"/>
       <c r="U2" s="72"/>
@@ -2864,24 +2873,24 @@
       <c r="AP2" s="28"/>
     </row>
     <row r="3" spans="1:42" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="89"/>
-      <c r="B3" s="90"/>
-      <c r="C3" s="90"/>
-      <c r="D3" s="90"/>
-      <c r="E3" s="90"/>
-      <c r="F3" s="91"/>
-      <c r="G3" s="91"/>
-      <c r="H3" s="104"/>
-      <c r="I3" s="104"/>
-      <c r="J3" s="104"/>
-      <c r="K3" s="104"/>
-      <c r="L3" s="91"/>
-      <c r="M3" s="91"/>
-      <c r="N3" s="104"/>
-      <c r="O3" s="104"/>
-      <c r="P3" s="104"/>
-      <c r="Q3" s="104"/>
-      <c r="R3" s="91"/>
+      <c r="A3" s="99"/>
+      <c r="B3" s="100"/>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="92"/>
+      <c r="G3" s="92"/>
+      <c r="H3" s="93"/>
+      <c r="I3" s="93"/>
+      <c r="J3" s="93"/>
+      <c r="K3" s="93"/>
+      <c r="L3" s="92"/>
+      <c r="M3" s="92"/>
+      <c r="N3" s="93"/>
+      <c r="O3" s="93"/>
+      <c r="P3" s="93"/>
+      <c r="Q3" s="93"/>
+      <c r="R3" s="92"/>
       <c r="S3" s="74"/>
       <c r="T3" s="74"/>
       <c r="U3" s="74"/>
@@ -2908,24 +2917,24 @@
       <c r="AP3" s="28"/>
     </row>
     <row r="4" spans="1:42" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="92"/>
-      <c r="B4" s="93"/>
-      <c r="C4" s="91"/>
-      <c r="D4" s="91"/>
-      <c r="E4" s="91"/>
-      <c r="F4" s="91"/>
-      <c r="G4" s="91"/>
-      <c r="H4" s="91"/>
-      <c r="I4" s="91"/>
-      <c r="J4" s="105"/>
-      <c r="K4" s="105"/>
-      <c r="L4" s="105"/>
-      <c r="M4" s="105"/>
-      <c r="N4" s="105"/>
-      <c r="O4" s="105"/>
-      <c r="P4" s="105"/>
-      <c r="Q4" s="105"/>
-      <c r="R4" s="105"/>
+      <c r="A4" s="101"/>
+      <c r="B4" s="102"/>
+      <c r="C4" s="92"/>
+      <c r="D4" s="92"/>
+      <c r="E4" s="92"/>
+      <c r="F4" s="92"/>
+      <c r="G4" s="92"/>
+      <c r="H4" s="92"/>
+      <c r="I4" s="92"/>
+      <c r="J4" s="94"/>
+      <c r="K4" s="94"/>
+      <c r="L4" s="94"/>
+      <c r="M4" s="94"/>
+      <c r="N4" s="94"/>
+      <c r="O4" s="94"/>
+      <c r="P4" s="94"/>
+      <c r="Q4" s="94"/>
+      <c r="R4" s="94"/>
       <c r="S4" s="76"/>
       <c r="T4" s="76"/>
       <c r="U4" s="76"/>
@@ -2952,19 +2961,19 @@
       <c r="AP4" s="28"/>
     </row>
     <row r="5" spans="1:42" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="94" t="s">
+      <c r="A5" s="103" t="s">
         <v>76</v>
       </c>
-      <c r="B5" s="95"/>
+      <c r="B5" s="104"/>
       <c r="C5" s="78" t="s">
         <v>204</v>
       </c>
-      <c r="D5" s="96"/>
-      <c r="E5" s="97"/>
-      <c r="F5" s="97"/>
-      <c r="G5" s="106"/>
-      <c r="H5" s="97"/>
-      <c r="I5" s="97"/>
+      <c r="D5" s="105"/>
+      <c r="E5" s="96"/>
+      <c r="F5" s="96"/>
+      <c r="G5" s="95"/>
+      <c r="H5" s="96"/>
+      <c r="I5" s="96"/>
       <c r="J5" s="30"/>
       <c r="K5" s="30"/>
       <c r="L5" s="30"/>
@@ -3088,34 +3097,34 @@
       <c r="AP7" s="28"/>
     </row>
     <row r="8" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A8" s="98"/>
-      <c r="B8" s="99"/>
-      <c r="C8" s="99"/>
-      <c r="D8" s="99"/>
-      <c r="E8" s="99"/>
-      <c r="F8" s="99"/>
-      <c r="G8" s="100"/>
-      <c r="H8" s="101" t="s">
+      <c r="A8" s="106"/>
+      <c r="B8" s="88"/>
+      <c r="C8" s="88"/>
+      <c r="D8" s="88"/>
+      <c r="E8" s="88"/>
+      <c r="F8" s="88"/>
+      <c r="G8" s="89"/>
+      <c r="H8" s="87" t="s">
         <v>77</v>
       </c>
-      <c r="I8" s="99"/>
-      <c r="J8" s="99"/>
-      <c r="K8" s="99"/>
-      <c r="L8" s="100"/>
-      <c r="M8" s="101" t="s">
+      <c r="I8" s="88"/>
+      <c r="J8" s="88"/>
+      <c r="K8" s="88"/>
+      <c r="L8" s="89"/>
+      <c r="M8" s="87" t="s">
         <v>78</v>
       </c>
-      <c r="N8" s="99"/>
-      <c r="O8" s="99"/>
-      <c r="P8" s="99"/>
-      <c r="Q8" s="100"/>
-      <c r="R8" s="101" t="s">
+      <c r="N8" s="88"/>
+      <c r="O8" s="88"/>
+      <c r="P8" s="88"/>
+      <c r="Q8" s="89"/>
+      <c r="R8" s="87" t="s">
         <v>79</v>
       </c>
-      <c r="S8" s="99"/>
-      <c r="T8" s="99"/>
-      <c r="U8" s="99"/>
-      <c r="V8" s="100"/>
+      <c r="S8" s="88"/>
+      <c r="T8" s="88"/>
+      <c r="U8" s="88"/>
+      <c r="V8" s="89"/>
       <c r="W8" s="36"/>
       <c r="X8" s="36"/>
       <c r="Y8" s="36"/>
@@ -3291,13 +3300,17 @@
       <c r="G11" s="67" t="s">
         <v>97</v>
       </c>
-      <c r="H11" s="67"/>
+      <c r="H11" s="67" t="s">
+        <v>97</v>
+      </c>
       <c r="I11" s="69" t="s">
-        <v>98</v>
+        <v>212</v>
       </c>
       <c r="J11" s="48"/>
       <c r="K11" s="49"/>
-      <c r="L11" s="50"/>
+      <c r="L11" s="107">
+        <v>44859</v>
+      </c>
       <c r="M11" s="51"/>
       <c r="N11" s="52"/>
       <c r="O11" s="48"/>
@@ -3351,13 +3364,17 @@
       <c r="G12" s="70" t="s">
         <v>97</v>
       </c>
-      <c r="H12" s="67"/>
+      <c r="H12" s="67" t="s">
+        <v>97</v>
+      </c>
       <c r="I12" s="69" t="s">
-        <v>98</v>
+        <v>212</v>
       </c>
       <c r="J12" s="52"/>
       <c r="K12" s="48"/>
-      <c r="L12" s="49"/>
+      <c r="L12" s="49">
+        <v>44859</v>
+      </c>
       <c r="M12" s="56"/>
       <c r="N12" s="52"/>
       <c r="O12" s="52"/>
@@ -3411,9 +3428,11 @@
       <c r="G13" s="58" t="s">
         <v>104</v>
       </c>
-      <c r="H13" s="67"/>
+      <c r="H13" s="67" t="s">
+        <v>97</v>
+      </c>
       <c r="I13" s="69" t="s">
-        <v>98</v>
+        <v>213</v>
       </c>
       <c r="J13" s="52"/>
       <c r="K13" s="48"/>
@@ -47139,16 +47158,16 @@
   </sheetData>
   <autoFilter ref="A9:AP73" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <mergeCells count="10">
+    <mergeCell ref="A2:F4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="A8:G8"/>
+    <mergeCell ref="H8:L8"/>
     <mergeCell ref="M8:Q8"/>
     <mergeCell ref="R8:V8"/>
     <mergeCell ref="G2:L4"/>
     <mergeCell ref="M2:R4"/>
     <mergeCell ref="G5:I5"/>
-    <mergeCell ref="A2:F4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="A8:G8"/>
-    <mergeCell ref="H8:L8"/>
   </mergeCells>
   <conditionalFormatting sqref="J9:J10 J12:J1000 J623:J1000 J749:J1000 J751:J1000 J753:J1000 J755:J1000 J757:J1000 J759:J1000 J761:J1000 J763:J1000 J765:J1000 J919:J1000 O9:O10 O12:O1000 O623:O1000 O749:O1000 O751:O1000 O753:O1000 O755:O1000 O757:O1000 O759:O1000 O761:O1000 O763:O1000 O765:O1000 O919:O1000">
     <cfRule type="cellIs" dxfId="46" priority="1" stopIfTrue="1" operator="equal">

</xml_diff>